<commit_message>
Validated power modelling for cyclists
</commit_message>
<xml_diff>
--- a/src/carpy/propulsion/data/cyclinganalytics_power.xlsx
+++ b/src/carpy/propulsion/data/cyclinganalytics_power.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/yr3g17_soton_ac_uk/Documents/Documents/Python/carpy/src/carpy/propulsion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_AD4DB114E441178AC67DF4E0B696ECB4693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7D581B4-890A-4481-BCE2-AA0D26453B0F}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="11_AD4DB114E441178AC67DF4E0B696ECB4693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1740E4F0-8024-4FD7-9EEB-63A47D2013EE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10316" windowHeight="10993" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>How does your cycling power output compare? — Cycling Analytics</t>
   </si>
@@ -72,7 +72,19 @@
     <t>Female Watts per kilogram</t>
   </si>
   <si>
-    <t>% / [s]</t>
+    <t>5s [W]</t>
+  </si>
+  <si>
+    <t>60s [W]</t>
+  </si>
+  <si>
+    <t>300s [W]</t>
+  </si>
+  <si>
+    <t>1200s [W]</t>
+  </si>
+  <si>
+    <t>percentile [%]</t>
   </si>
 </sst>
 </file>
@@ -403,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -461,27 +473,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C8BE84-EF0C-4E6C-A12B-9BB030DC8113}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1">
-        <v>5</v>
-      </c>
-      <c r="C1">
-        <v>60</v>
-      </c>
-      <c r="D1">
-        <v>300</v>
-      </c>
-      <c r="E1">
-        <v>1200</v>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -715,27 +725,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E1EFCD-5AA7-4C70-8154-C6F3131508DF}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1">
-        <v>5</v>
-      </c>
-      <c r="C1">
-        <v>60</v>
-      </c>
-      <c r="D1">
-        <v>300</v>
-      </c>
-      <c r="E1">
-        <v>1200</v>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -968,27 +976,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E6E598-1295-4248-9F5E-946714FE54B9}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1">
-        <v>5</v>
-      </c>
-      <c r="C1">
-        <v>60</v>
-      </c>
-      <c r="D1">
-        <v>300</v>
-      </c>
-      <c r="E1">
-        <v>1200</v>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1187,27 +1193,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52349CC-E3BF-427A-96BE-A00773D50195}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1">
-        <v>5</v>
-      </c>
-      <c r="C1">
-        <v>60</v>
-      </c>
-      <c r="D1">
-        <v>300</v>
-      </c>
-      <c r="E1">
-        <v>1200</v>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>